<commit_message>
Update PM05 Tidsregistrering for Mik.xlsx
co-author: ingen
reviewer: ingen
</commit_message>
<xml_diff>
--- a/08 Project Management/Tidsregistrering/PM05 Tidsregistrering for Mik.xlsx
+++ b/08 Project Management/Tidsregistrering/PM05 Tidsregistrering for Mik.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikpe\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F521FB44-3323-4750-A2E6-05EE14B5A3E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C106FBFC-DD1D-44AA-9A10-87C980926C1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9648" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
   <si>
     <t>Tidsregistrering af (Navn)</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Timer i alt</t>
   </si>
   <si>
-    <t>Udarbejdelse af DOM08 med anders</t>
-  </si>
-  <si>
     <t>Business-Process Analyst</t>
   </si>
   <si>
@@ -175,6 +172,21 @@
   </si>
   <si>
     <t>Kundemøde</t>
+  </si>
+  <si>
+    <t>Udarbejdelse af SSD01 med Tommy</t>
+  </si>
+  <si>
+    <t>Review ad AD01 med Matias</t>
+  </si>
+  <si>
+    <t>Udarbejdelse af DOM08 med Anders</t>
+  </si>
+  <si>
+    <t>Review af DOM01 med Toke</t>
+  </si>
+  <si>
+    <t>Udarbejdelse af iterationsplan 2</t>
   </si>
 </sst>
 </file>
@@ -757,7 +769,7 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -811,10 +823,10 @@
     </row>
     <row r="3" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>42</v>
       </c>
       <c r="C3" s="12">
         <v>43885</v>
@@ -837,10 +849,10 @@
     </row>
     <row r="4" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A4" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="12">
         <v>43885</v>
@@ -863,10 +875,10 @@
     </row>
     <row r="5" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A5" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="12">
         <v>43885</v>
@@ -889,10 +901,10 @@
     </row>
     <row r="6" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A6" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="12">
         <v>43885</v>
@@ -915,10 +927,10 @@
     </row>
     <row r="7" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A7" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="12">
         <v>43885</v>
@@ -940,59 +952,107 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
+      <c r="A8" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="15">
+        <v>43886</v>
+      </c>
+      <c r="D8" s="16">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E8" s="16">
+        <v>0.42708333333333331</v>
+      </c>
       <c r="F8" s="21"/>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.291666666666663E-2</v>
       </c>
       <c r="H8" s="1">
         <f>SUM(G$3:G8)</f>
-        <v>0.25</v>
+        <v>0.32291666666666663</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
+      <c r="A9" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="15">
+        <v>43886</v>
+      </c>
+      <c r="D9" s="16">
+        <v>0.4375</v>
+      </c>
+      <c r="E9" s="16">
+        <v>0.46875</v>
+      </c>
       <c r="F9" s="21"/>
       <c r="G9" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
       <c r="H9" s="1">
         <f>SUM(G$3:G9)</f>
-        <v>0.25</v>
+        <v>0.35416666666666663</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
+      <c r="A10" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="15">
+        <v>43886</v>
+      </c>
+      <c r="D10" s="16">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="E10" s="16">
+        <v>0.53819444444444442</v>
+      </c>
       <c r="F10" s="21"/>
       <c r="G10" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
       <c r="H10" s="1">
         <f>SUM(G$3:G10)</f>
-        <v>0.25</v>
+        <v>0.38541666666666663</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
+      <c r="A11" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="15">
+        <v>43886</v>
+      </c>
+      <c r="D11" s="16">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="E11" s="16">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="F11" s="21"/>
       <c r="G11" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.15625</v>
       </c>
       <c r="H11" s="1">
         <f>SUM(G$3:G11)</f>
-        <v>0.25</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1006,7 +1066,7 @@
       </c>
       <c r="H12" s="1">
         <f>SUM(G$3:G12)</f>
-        <v>0.25</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1020,7 +1080,7 @@
       </c>
       <c r="H13" s="1">
         <f>SUM(G$3:G13)</f>
-        <v>0.25</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1032,7 +1092,7 @@
       </c>
       <c r="H14" s="1">
         <f>SUM(G$3:G14)</f>
-        <v>0.25</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1044,7 +1104,7 @@
       </c>
       <c r="H15" s="1">
         <f>SUM(G$3:G15)</f>
-        <v>0.25</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1056,7 +1116,7 @@
       </c>
       <c r="H16" s="1">
         <f>SUM(G$3:G16)</f>
-        <v>0.25</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="17" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1068,7 +1128,7 @@
       </c>
       <c r="H17" s="1">
         <f>SUM(G$3:G17)</f>
-        <v>0.25</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="18" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1080,7 +1140,7 @@
       </c>
       <c r="H18" s="1">
         <f>SUM(G$3:G18)</f>
-        <v>0.25</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="19" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1092,7 +1152,7 @@
       </c>
       <c r="H19" s="1">
         <f>SUM(G$3:G19)</f>
-        <v>0.25</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="20" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1104,7 +1164,7 @@
       </c>
       <c r="H20" s="1">
         <f>SUM(G$3:G20)</f>
-        <v>0.25</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="21" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1116,7 +1176,7 @@
       </c>
       <c r="H21" s="1">
         <f>SUM(G$3:G21)</f>
-        <v>0.25</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="22" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1128,7 +1188,7 @@
       </c>
       <c r="H22" s="1">
         <f>SUM(G$3:G22)</f>
-        <v>0.25</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="23" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1140,7 +1200,7 @@
       </c>
       <c r="H23" s="1">
         <f>SUM(G$3:G23)</f>
-        <v>0.25</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="24" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1152,7 +1212,7 @@
       </c>
       <c r="H24" s="1">
         <f>SUM(G$3:G24)</f>
-        <v>0.25</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="25" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1163,7 +1223,7 @@
       </c>
       <c r="H25" s="1">
         <f>SUM(G$3:G25)</f>
-        <v>0.25</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="26" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1174,7 +1234,7 @@
       </c>
       <c r="H26" s="1">
         <f>SUM(G$3:G26)</f>
-        <v>0.25</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="27" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1185,7 +1245,7 @@
       </c>
       <c r="H27" s="1">
         <f>SUM(G$3:G27)</f>
-        <v>0.25</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="28" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1196,7 +1256,7 @@
       </c>
       <c r="H28" s="1">
         <f>SUM(G$3:G28)</f>
-        <v>0.25</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="29" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1207,7 +1267,7 @@
       </c>
       <c r="H29" s="1">
         <f>SUM(G$3:G29)</f>
-        <v>0.25</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="30" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1218,7 +1278,7 @@
       </c>
       <c r="H30" s="1">
         <f>SUM(G$3:G30)</f>
-        <v>0.25</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="31" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1229,7 +1289,7 @@
       </c>
       <c r="H31" s="1">
         <f>SUM(G$3:G31)</f>
-        <v>0.25</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="32" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1240,7 +1300,7 @@
       </c>
       <c r="H32" s="1">
         <f>SUM(G$3:G32)</f>
-        <v>0.25</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.3">

</xml_diff>